<commit_message>
trans/AVPC updating 3.3.1 file to EU-specific data
</commit_message>
<xml_diff>
--- a/InputData/trans/AVPC/Annual Vehicle Parking Costs.xlsx
+++ b/InputData/trans/AVPC/Annual Vehicle Parking Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\trans\AVPC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire Trevisan\Dropbox (Energy Innovation)\Documents\GitHub\eps-eu\InputData\trans\AVPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE5C0E1-FFC8-4760-BC76-F4AD6505844A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3744D266-91B6-4406-93E4-2DE0E89D456A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12870" yWindow="1470" windowWidth="18165" windowHeight="21135" xr2:uid="{7A96142A-95FE-491D-9737-978D460925CE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A96142A-95FE-491D-9737-978D460925CE}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>AVPC Annual Vehicle Parking Costs</t>
   </si>
@@ -47,87 +47,21 @@
     <t>INRIX</t>
   </si>
   <si>
-    <t>Parking Costs in Major Cities</t>
-  </si>
-  <si>
-    <t>https://inrix.com/press-releases/cod-us/</t>
-  </si>
-  <si>
-    <t>New INRIX Study Finds Parking is the Largest Cost of Driving</t>
-  </si>
-  <si>
-    <t>Time Spent Looking for Parking</t>
-  </si>
-  <si>
-    <t>New York City</t>
-  </si>
-  <si>
-    <t>Los Angeles</t>
-  </si>
-  <si>
-    <t>San Francisco</t>
-  </si>
-  <si>
-    <t>Washington DC</t>
-  </si>
-  <si>
-    <t>Seattle</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>Atlanta</t>
-  </si>
-  <si>
-    <t>Dallas</t>
-  </si>
-  <si>
-    <t>U.S. Average</t>
-  </si>
-  <si>
-    <t>Detroit</t>
-  </si>
-  <si>
-    <t>Cost (2017 USD/yr)</t>
-  </si>
-  <si>
     <t>Cost to Time Ratio</t>
   </si>
   <si>
     <t>Time Spent (hr/yr)</t>
   </si>
   <si>
-    <t>https://www.usatoday.com/story/money/2017/07/12/parking-pain-causes-financial-and-personal-strain/467637001/</t>
-  </si>
-  <si>
-    <t>Drivers spend an average of 17 hours a year searching for parking spots</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>INRIX has annual parking costs (per driver) for 10 major U.S. cities.</t>
-  </si>
-  <si>
-    <t>However, this does not reflect a nation-wide average, which includes</t>
-  </si>
-  <si>
     <t>many smaller cities, towns and rural areas.</t>
   </si>
   <si>
     <t>INRIX also has the annual amount of time spent looking for parking</t>
   </si>
   <si>
-    <t>in the same 10 major U.S. cities, and a national average for the whole U.S.</t>
-  </si>
-  <si>
-    <t>In order to estimate parking costs for the whole U.S., we assume that the</t>
-  </si>
-  <si>
     <t>amount of money paid for parking and the amount of time spent looking</t>
   </si>
   <si>
@@ -137,9 +71,6 @@
     <t>outstrips supply, causing longer time spent looking for parking).</t>
   </si>
   <si>
-    <t>We establish an average ratio of cost-to-time for the ten major cities</t>
-  </si>
-  <si>
     <t>and apply this ratio to the national average time spent looking for parking</t>
   </si>
   <si>
@@ -180,6 +111,72 @@
   </si>
   <si>
     <t>(as non-free parking, and parking rates, would rise in situations where demand</t>
+  </si>
+  <si>
+    <t>Frankfurt</t>
+  </si>
+  <si>
+    <t>Essen</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Dusseldorf</t>
+  </si>
+  <si>
+    <t>Cologne</t>
+  </si>
+  <si>
+    <t>Dortmund</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Stuttgart</t>
+  </si>
+  <si>
+    <t>Munich</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Germany Average</t>
+  </si>
+  <si>
+    <t>2017 Euro to 2017 USD</t>
+  </si>
+  <si>
+    <t>Cost (2017 Euro/yr)</t>
+  </si>
+  <si>
+    <t>The Impact of Parking Pain in the US, UK and Germany</t>
+  </si>
+  <si>
+    <t>Parking Costs in Major Cities and Time Spent Looking for Parking</t>
+  </si>
+  <si>
+    <t>https://www2.inrix.com/research-parking-2017</t>
+  </si>
+  <si>
+    <t>INRIX has annual parking costs (per driver) for 10 major U.S., UK, and German cities.</t>
+  </si>
+  <si>
+    <t>However, this does not reflect a nation-wide average (or EU-wide average), which includes</t>
+  </si>
+  <si>
+    <t>in the same 10 major cities, and a national average for the countries.</t>
+  </si>
+  <si>
+    <t>In order to estimate parking costs for the whole EU, we assume that the</t>
+  </si>
+  <si>
+    <t>We establish an average ratio of cost-to-time for the ten major cities in Germany,</t>
+  </si>
+  <si>
+    <t>assume this ratio and the national average time spent looking for parking in Germany is consistent across the EU,</t>
   </si>
 </sst>
 </file>
@@ -187,7 +184,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -258,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -290,22 +287,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>44707</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>17146</xdr:rowOff>
+      <xdr:rowOff>139934</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FCEBA2D-5F2E-4120-A31C-AED7F058C353}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B3A3A0C-633B-E79C-00F4-0D5B5F77D43C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -314,21 +311,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4867275" y="390526"/>
-          <a:ext cx="4572000" cy="4198620"/>
+          <a:off x="5562600" y="0"/>
+          <a:ext cx="5010407" cy="4489684"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -637,163 +628,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A3C504-1517-4439-8CB6-64CD86FC1AAC}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>1.1304000000000001</v>
+      </c>
+      <c r="B31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>0.93700000000000006</v>
-      </c>
-      <c r="B34" t="s">
-        <v>37</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{95049637-93AE-4459-97A9-ED566F862A07}"/>
-    <hyperlink ref="B13" r:id="rId2" xr:uid="{0B4DBBE0-E563-4FF9-9E60-2E166BC78EA1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -801,187 +778,189 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EEAD45-8CD8-474E-BA40-724705BC176E}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.7265625" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>5395</v>
+        <v>1410</v>
       </c>
       <c r="C2">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="D2" s="6">
         <f>B2/C2</f>
-        <v>50.420560747663551</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.692307692307693</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>2405</v>
+        <v>1390</v>
       </c>
       <c r="C3">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D11" si="0">B3/C3</f>
-        <v>28.294117647058822</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.71875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B4">
-        <v>2801</v>
+        <v>1358</v>
       </c>
       <c r="C4">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="0"/>
-        <v>33.746987951807228</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.903225806451612</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B5">
-        <v>2170</v>
+        <v>1337</v>
       </c>
       <c r="C5">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="0"/>
-        <v>33.384615384615387</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.918032786885245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B6">
-        <v>1274</v>
+        <v>1302</v>
       </c>
       <c r="C6">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="0"/>
-        <v>21.96551724137931</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B7">
-        <v>2096</v>
+        <v>1239</v>
       </c>
       <c r="C7">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="0"/>
-        <v>37.428571428571431</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.736842105263158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B8">
-        <v>2045</v>
+        <v>1139</v>
       </c>
       <c r="C8">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>38.584905660377359</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.903846153846153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B9">
-        <v>872</v>
+        <v>1136</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
-        <v>17.440000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.846153846153847</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B10">
-        <v>723</v>
+        <v>1092</v>
       </c>
       <c r="C10">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" si="0"/>
-        <v>15.0625</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B11">
-        <v>815</v>
+        <v>1065</v>
       </c>
       <c r="C11">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" si="0"/>
-        <v>23.285714285714285</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.73469387755102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B12" s="8">
         <f>C12*AVERAGE(D2:D11)</f>
-        <v>509.34293359021859</v>
+        <v>893.77479430068081</v>
       </c>
       <c r="C12">
-        <v>17</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -997,40 +976,42 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="3" width="13.42578125" customWidth="1"/>
+    <col min="2" max="3" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B2" s="7">
-        <f>Data!B12*About!A34</f>
-        <v>477.25432877403483</v>
+        <f>Data!B12*About!A31*About!A30</f>
+        <v>946.67267674640789</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="B3" s="7">
         <v>0</v>
@@ -1039,9 +1020,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1050,9 +1031,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1061,9 +1042,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1072,9 +1053,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
Uploading AVPC data file
</commit_message>
<xml_diff>
--- a/InputData/trans/AVPC/Annual Vehicle Parking Costs.xlsx
+++ b/InputData/trans/AVPC/Annual Vehicle Parking Costs.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\trans\AVPC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire Trevisan\Dropbox (Energy Innovation)\Documents\GitHub\eps-eu\InputData\trans\AVPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE5C0E1-FFC8-4760-BC76-F4AD6505844A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{3744D266-91B6-4406-93E4-2DE0E89D456A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95B597F3-385C-4510-BE93-1FFF2105CBD2}"/>
   <bookViews>
-    <workbookView xWindow="12870" yWindow="1470" windowWidth="18165" windowHeight="21135" xr2:uid="{7A96142A-95FE-491D-9737-978D460925CE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{7A96142A-95FE-491D-9737-978D460925CE}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="AVPC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,6 +29,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>AVPC Annual Vehicle Parking Costs</t>
   </si>
@@ -44,112 +46,112 @@
     <t>Source:</t>
   </si>
   <si>
+    <t>Parking Costs in Major Cities and Time Spent Looking for Parking</t>
+  </si>
+  <si>
     <t>INRIX</t>
   </si>
   <si>
-    <t>Parking Costs in Major Cities</t>
-  </si>
-  <si>
-    <t>https://inrix.com/press-releases/cod-us/</t>
-  </si>
-  <si>
-    <t>New INRIX Study Finds Parking is the Largest Cost of Driving</t>
-  </si>
-  <si>
-    <t>Time Spent Looking for Parking</t>
-  </si>
-  <si>
-    <t>New York City</t>
-  </si>
-  <si>
-    <t>Los Angeles</t>
-  </si>
-  <si>
-    <t>San Francisco</t>
-  </si>
-  <si>
-    <t>Washington DC</t>
-  </si>
-  <si>
-    <t>Seattle</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>Atlanta</t>
-  </si>
-  <si>
-    <t>Dallas</t>
-  </si>
-  <si>
-    <t>U.S. Average</t>
-  </si>
-  <si>
-    <t>Detroit</t>
-  </si>
-  <si>
-    <t>Cost (2017 USD/yr)</t>
+    <t>The Impact of Parking Pain in the US, UK and Germany</t>
+  </si>
+  <si>
+    <t>https://www2.inrix.com/research-parking-2017</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>INRIX has annual parking costs (per driver) for 10 major U.S., UK, and German cities.</t>
+  </si>
+  <si>
+    <t>However, this does not reflect a nation-wide average (or EU-wide average), which includes</t>
+  </si>
+  <si>
+    <t>many smaller cities, towns and rural areas.</t>
+  </si>
+  <si>
+    <t>INRIX also has the annual amount of time spent looking for parking</t>
+  </si>
+  <si>
+    <t>in the same 10 major cities, and a national average for the countries.</t>
+  </si>
+  <si>
+    <t>In order to estimate parking costs for the whole EU, we assume that the</t>
+  </si>
+  <si>
+    <t>amount of money paid for parking and the amount of time spent looking</t>
+  </si>
+  <si>
+    <t>for parking in a given place are directly proportionate to each other</t>
+  </si>
+  <si>
+    <t>(as non-free parking, and parking rates, would rise in situations where demand</t>
+  </si>
+  <si>
+    <t>outstrips supply, causing longer time spent looking for parking).</t>
+  </si>
+  <si>
+    <t>We establish an average ratio of cost-to-time for the ten major cities in Germany,</t>
+  </si>
+  <si>
+    <t>assume this ratio and the national average time spent looking for parking in Germany is consistent across the EU,</t>
+  </si>
+  <si>
+    <t>and apply this ratio to the national average time spent looking for parking</t>
+  </si>
+  <si>
+    <t>to obtain a national average parking cost.</t>
+  </si>
+  <si>
+    <t>Conversion Factor</t>
+  </si>
+  <si>
+    <t>2017 to 2012 USD</t>
+  </si>
+  <si>
+    <t>2017 Euro to 2017 USD</t>
+  </si>
+  <si>
+    <t>Cost (2017 Euro/yr)</t>
+  </si>
+  <si>
+    <t>Time Spent (hr/yr)</t>
   </si>
   <si>
     <t>Cost to Time Ratio</t>
   </si>
   <si>
-    <t>Time Spent (hr/yr)</t>
-  </si>
-  <si>
-    <t>https://www.usatoday.com/story/money/2017/07/12/parking-pain-causes-financial-and-personal-strain/467637001/</t>
-  </si>
-  <si>
-    <t>Drivers spend an average of 17 hours a year searching for parking spots</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>INRIX has annual parking costs (per driver) for 10 major U.S. cities.</t>
-  </si>
-  <si>
-    <t>However, this does not reflect a nation-wide average, which includes</t>
-  </si>
-  <si>
-    <t>many smaller cities, towns and rural areas.</t>
-  </si>
-  <si>
-    <t>INRIX also has the annual amount of time spent looking for parking</t>
-  </si>
-  <si>
-    <t>in the same 10 major U.S. cities, and a national average for the whole U.S.</t>
-  </si>
-  <si>
-    <t>In order to estimate parking costs for the whole U.S., we assume that the</t>
-  </si>
-  <si>
-    <t>amount of money paid for parking and the amount of time spent looking</t>
-  </si>
-  <si>
-    <t>for parking in a given place are directly proportionate to each other</t>
-  </si>
-  <si>
-    <t>outstrips supply, causing longer time spent looking for parking).</t>
-  </si>
-  <si>
-    <t>We establish an average ratio of cost-to-time for the ten major cities</t>
-  </si>
-  <si>
-    <t>and apply this ratio to the national average time spent looking for parking</t>
-  </si>
-  <si>
-    <t>to obtain a national average parking cost.</t>
-  </si>
-  <si>
-    <t>Conversion Factor</t>
-  </si>
-  <si>
-    <t>2017 to 2012 USD</t>
+    <t>Frankfurt</t>
+  </si>
+  <si>
+    <t>Essen</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Dusseldorf</t>
+  </si>
+  <si>
+    <t>Cologne</t>
+  </si>
+  <si>
+    <t>Dortmund</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Stuttgart</t>
+  </si>
+  <si>
+    <t>Munich</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Germany Average</t>
   </si>
   <si>
     <t>2012 USD/year</t>
@@ -177,9 +179,6 @@
   </si>
   <si>
     <t>motorbikes</t>
-  </si>
-  <si>
-    <t>(as non-free parking, and parking rates, would rise in situations where demand</t>
   </si>
 </sst>
 </file>
@@ -187,9 +186,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,7 +257,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -269,8 +268,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -289,23 +288,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>17146</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FCEBA2D-5F2E-4120-A31C-AED7F058C353}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B3A3A0C-633B-E79C-00F4-0D5B5F77D43C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -314,21 +313,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4867275" y="390526"/>
-          <a:ext cx="4572000" cy="4198620"/>
+          <a:off x="4619625" y="0"/>
+          <a:ext cx="8020050" cy="6991350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -637,163 +630,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A3C504-1517-4439-8CB6-64CD86FC1AAC}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="2" max="2" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="B5" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="B30" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>1.1304000000000001</v>
+      </c>
+      <c r="B31" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>0.93700000000000006</v>
-      </c>
-      <c r="B34" t="s">
-        <v>37</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{95049637-93AE-4459-97A9-ED566F862A07}"/>
-    <hyperlink ref="B13" r:id="rId2" xr:uid="{0B4DBBE0-E563-4FF9-9E60-2E166BC78EA1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -801,9 +780,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EEAD45-8CD8-474E-BA40-724705BC176E}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
@@ -811,177 +792,177 @@
     <col min="4" max="4" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="29.1">
       <c r="B1" s="5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B2">
-        <v>5395</v>
+        <v>1410</v>
       </c>
       <c r="C2">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="D2" s="6">
         <f>B2/C2</f>
-        <v>50.420560747663551</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.692307692307693</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B3">
-        <v>2405</v>
+        <v>1390</v>
       </c>
       <c r="C3">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D11" si="0">B3/C3</f>
-        <v>28.294117647058822</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.71875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B4">
-        <v>2801</v>
+        <v>1358</v>
       </c>
       <c r="C4">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="0"/>
-        <v>33.746987951807228</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.903225806451612</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B5">
-        <v>2170</v>
+        <v>1337</v>
       </c>
       <c r="C5">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="0"/>
-        <v>33.384615384615387</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.918032786885245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B6">
-        <v>1274</v>
+        <v>1302</v>
       </c>
       <c r="C6">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="0"/>
-        <v>21.96551724137931</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B7">
-        <v>2096</v>
+        <v>1239</v>
       </c>
       <c r="C7">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="0"/>
-        <v>37.428571428571431</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.736842105263158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B8">
-        <v>2045</v>
+        <v>1139</v>
       </c>
       <c r="C8">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>38.584905660377359</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.903846153846153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B9">
-        <v>872</v>
+        <v>1136</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
-        <v>17.440000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.846153846153847</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B10">
-        <v>723</v>
+        <v>1092</v>
       </c>
       <c r="C10">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" si="0"/>
-        <v>15.0625</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B11">
-        <v>815</v>
+        <v>1065</v>
       </c>
       <c r="C11">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" si="0"/>
-        <v>23.285714285714285</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21.73469387755102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B12" s="8">
         <f>C12*AVERAGE(D2:D11)</f>
-        <v>509.34293359021859</v>
+        <v>893.77479430068081</v>
       </c>
       <c r="C12">
-        <v>17</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -997,15 +978,17 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="3" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="9" t="s">
         <v>38</v>
       </c>
@@ -1016,19 +999,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="7">
-        <f>Data!B12*About!A34</f>
-        <v>477.25432877403483</v>
+        <f>Data!B12*About!A31*About!A30</f>
+        <v>946.67267674640789</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
@@ -1039,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>43</v>
       </c>
@@ -1050,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -1061,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
@@ -1072,7 +1055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
@@ -1086,4 +1069,265 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
+    <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <xsd:import namespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="00484652-42e1-479e-92f4-fb0efddcdf60" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="eca5b831-c3dc-41cf-bd85-218b82cecb21" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="21" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c5b79d03-3bfd-4c46-9947-056a2403f6c9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3838E1C8-C204-4D68-8F62-67C6955735C1}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDA73603-F64D-4189-8A40-BEF3F64F23EF}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C0803B-FDDD-49AD-8B47-502767FA6486}"/>
 </file>
</xml_diff>